<commit_message>
Batch module update commit
</commit_message>
<xml_diff>
--- a/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
+++ b/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senth\eclipse-workspace\Team6_Phase2_LMSAPIRestAssured\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BC0FDA-4CB7-4459-8B21-62D0C68FFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3266E7-0477-42BE-9AC3-AF2B782677FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LMS_valid_dataFinalUpdate_data1" sheetId="1" r:id="rId1"/>
+    <sheet name="Batchmodule_invaliddata" sheetId="2" r:id="rId2"/>
+    <sheet name="Batchmodule_validData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>userComments</t>
   </si>
@@ -119,6 +121,45 @@
   </si>
   <si>
     <t>testSd02121@gmail.com</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchName</t>
+  </si>
+  <si>
+    <t>batchNoOfClasses</t>
+  </si>
+  <si>
+    <t>batchStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>SDET Testing API Services</t>
+  </si>
+  <si>
+    <t>March24-APITeam-SDET-507</t>
+  </si>
+  <si>
+    <t>March24-Digital-Warriors-03</t>
+  </si>
+  <si>
+    <t>March24-Digital-Warriors-01</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Program March24-APITeam-SDET-507 with Batch-March24-Digital-Warriors-01 already exists: ; Please give a different batch Name or Choose a different Program</t>
+  </si>
+  <si>
+    <t>success</t>
   </si>
 </sst>
 </file>
@@ -992,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,6 +1042,9 @@
     <col min="12" max="12" width="22.140625" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
     <col min="14" max="14" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
     <col min="54" max="54" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1122,4 +1166,137 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFE32FC-9E74-4324-9BC0-13F8F9AFBD45}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>16614</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A270C26-81B4-4C77-A071-4D7CB6303311}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>16614</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATED usermodule -merged by vani
</commit_message>
<xml_diff>
--- a/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
+++ b/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team6_RestAssuredAPI\Users\senth\eclipse-workspace\Team6_Phase2_LMSAPIRestAssured\src\test\resources\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef72ffeab5838379/Desktop/Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52064983-696E-4EDF-BE22-3EAD3CA1B2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{4FE9F826-4508-4007-9AA4-54A2112DD4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046BF60B-6792-4B92-B3F0-F9B0E640BC56}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>userComments</t>
   </si>
@@ -167,13 +167,25 @@
   </si>
   <si>
     <t>userID</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatchStatus</t>
+  </si>
+  <si>
+    <t>INACTIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +333,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -665,10 +683,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,10 +1086,13 @@
     <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1131,8 +1153,17 @@
       <c r="T1" t="s">
         <v>48</v>
       </c>
+      <c r="U1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>19</v>
       </c>
@@ -1157,8 +1188,17 @@
       <c r="T2" t="s">
         <v>23</v>
       </c>
+      <c r="U2">
+        <v>16224</v>
+      </c>
+      <c r="V2">
+        <v>8652</v>
+      </c>
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O3" t="s">
         <v>17</v>
       </c>
@@ -1174,8 +1214,17 @@
       <c r="T3" t="s">
         <v>27</v>
       </c>
+      <c r="U3">
+        <v>16210</v>
+      </c>
+      <c r="V3">
+        <v>8465</v>
+      </c>
+      <c r="W3" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O4" t="s">
         <v>29</v>
       </c>
@@ -1192,7 +1241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O5" t="s">
         <v>32</v>
       </c>
@@ -1209,7 +1258,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>19</v>
       </c>
@@ -1249,7 +1298,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>37</v>
       </c>
@@ -1283,7 +1332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>31</v>
       </c>
@@ -1314,7 +1363,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Ashwini Program module commit
</commit_message>
<xml_diff>
--- a/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
+++ b/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
@@ -8,21 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senth\eclipse-workspace\Team6_Phase2_LMSAPIRestAssured\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3266E7-0477-42BE-9AC3-AF2B782677FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7288FDFB-94B1-484D-9286-AA20C3DEB9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LMS_valid_dataFinalUpdate_data1" sheetId="1" r:id="rId1"/>
-    <sheet name="Batchmodule_invaliddata" sheetId="2" r:id="rId2"/>
-    <sheet name="Batchmodule_validData" sheetId="3" r:id="rId3"/>
+    <sheet name="Inactive_pgmid" sheetId="5" r:id="rId2"/>
+    <sheet name="DeletebyID" sheetId="6" r:id="rId3"/>
+    <sheet name="GetbyName" sheetId="7" r:id="rId4"/>
+    <sheet name="Batchmodule_Existingdata" sheetId="2" r:id="rId5"/>
+    <sheet name="Invaliddata" sheetId="4" r:id="rId6"/>
+    <sheet name="Batchmodule_validData" sheetId="3" r:id="rId7"/>
+    <sheet name="Update_put" sheetId="8" r:id="rId8"/>
+    <sheet name="POST_ProgramModule" sheetId="9" r:id="rId9"/>
+    <sheet name="GET_ProgramModule" sheetId="11" r:id="rId10"/>
+    <sheet name="PUT_ProgramModule" sheetId="12" r:id="rId11"/>
+    <sheet name="DELETE_ProgramModule" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="168">
   <si>
     <t>userComments</t>
   </si>
@@ -160,13 +169,848 @@
   </si>
   <si>
     <t>success</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>March24-TechGeeks-SDET-SDET01-2111</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>Analyst54</t>
+  </si>
+  <si>
+    <t>March24-Digital-Warriors-06</t>
+  </si>
+  <si>
+    <t>March24-Digital-Warriors-07</t>
+  </si>
+  <si>
+    <t>testpgmbatch21</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>endpoint</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>baseURI</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>create a program with valid endpoint and request body with Authorization</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>/saveprogram</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Selenium Advanced Program1</t>
+  </si>
+  <si>
+    <t>AdvSel1</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>201 Created Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> with response body.</t>
+    </r>
+  </si>
+  <si>
+    <t>Selenium Advanced Program2</t>
+  </si>
+  <si>
+    <t>AdvSel2</t>
+  </si>
+  <si>
+    <t>create a program with valid endpoint and request body without Authorization</t>
+  </si>
+  <si>
+    <t>NoAuth</t>
+  </si>
+  <si>
+    <t>Selenium Advanced Program</t>
+  </si>
+  <si>
+    <t>AdvSel3</t>
+  </si>
+  <si>
+    <t>Admin receives 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>create a program with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/saveprograms</t>
+  </si>
+  <si>
+    <t>AdvSel4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">404 not found </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with message and boolean success details</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">create a program with already existing program name </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with message and boolean success details</t>
+    </r>
+  </si>
+  <si>
+    <t>create a program with invalid method</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>AdvSel5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">405 Method Not Allowed </t>
+    </r>
+  </si>
+  <si>
+    <t>create a program with invalid request body</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status</t>
+    </r>
+  </si>
+  <si>
+    <t>create a program with missing values in the request body</t>
+  </si>
+  <si>
+    <t>AdvSel6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">create a program with missing additional field </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AdvSel7</t>
+  </si>
+  <si>
+    <t>Admin receives 200 ok</t>
+  </si>
+  <si>
+    <t>to retrieve all programs with valid Endpoint</t>
+  </si>
+  <si>
+    <t>/allPrograms</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>200 OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with response body.                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t>to retrieve all programs with invalid Endpoint</t>
+  </si>
+  <si>
+    <t>/allProgram</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">404 not found </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with error message</t>
+    </r>
+  </si>
+  <si>
+    <t>to retrieve all programs with invalid Method</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">405 Method Not Allowed </t>
+    </r>
+  </si>
+  <si>
+    <t>to retrieve all programs without Authorization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin receives 401 Status with response body as Unauthorized                                  </t>
+  </si>
+  <si>
+    <t>to retrieve a program with valid program ID</t>
+  </si>
+  <si>
+    <t>/programs/{programId}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>200 OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with response body.                                                          </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">to retrieve a program with invalid program ID </t>
+  </si>
+  <si>
+    <t>/programs/{invalidprogramId}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Admin receives</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 404 Not Found</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with message and boolean success details</t>
+    </r>
+  </si>
+  <si>
+    <t>to retrieve a program with invalid baseURI</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>to retrieve a program without Authorization</t>
+  </si>
+  <si>
+    <t>to retrieve a program with invalid Endpoint</t>
+  </si>
+  <si>
+    <t>/progra/{programId}</t>
+  </si>
+  <si>
+    <t>to retrieve all programs with users with valid Endpoint</t>
+  </si>
+  <si>
+    <t>/allProgramsWithUsers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>200 OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with response body.                                                        </t>
+    </r>
+  </si>
+  <si>
+    <t>to retrieve all programs with users with invalid Endpoint</t>
+  </si>
+  <si>
+    <t>/allProgramsWithUser</t>
+  </si>
+  <si>
+    <t>to retrieve all programs with users with invalid Method</t>
+  </si>
+  <si>
+    <t>to retrieve all programs with users without Authorization</t>
+  </si>
+  <si>
+    <t>RequestBody</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>to update a program with valid programID endpoint  and valid request body</t>
+  </si>
+  <si>
+    <t>/putprogram/{programId}</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Selenium Advanced Program Updated</t>
+  </si>
+  <si>
+    <t>{programId}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>200 OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with updated value in response body.                                           </t>
+    </r>
+  </si>
+  <si>
+    <t>to update a program with invalid programID endpoint  and valid request body</t>
+  </si>
+  <si>
+    <t>/putprogram/{invalidprogramId}</t>
+  </si>
+  <si>
+    <t>{invalidprogramId}</t>
+  </si>
+  <si>
+    <t>to update a program with invalid request body</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Admin receives</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Status with message and boolean success details</t>
+    </r>
+  </si>
+  <si>
+    <t>to update a program without request body</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Admin receives</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 400 Bad Request </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Status with message and boolean success details</t>
+    </r>
+  </si>
+  <si>
+    <t>to update a program with invalid baseURI</t>
+  </si>
+  <si>
+    <t>to update a program with invalid method</t>
+  </si>
+  <si>
+    <t>to update a program without Authorization</t>
+  </si>
+  <si>
+    <t>to update a program with  Valid program Name and request body</t>
+  </si>
+  <si>
+    <t>/program/{programName}</t>
+  </si>
+  <si>
+    <t>Updated Selenium Advanced</t>
+  </si>
+  <si>
+    <t>{programName}</t>
+  </si>
+  <si>
+    <t>to update a program with  invalid program Name and request body</t>
+  </si>
+  <si>
+    <t>/program/{invalidprogramName}</t>
+  </si>
+  <si>
+    <t>{invalidprogramName}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to update a program using valid program name - missing mandatory fields in request body </t>
+  </si>
+  <si>
+    <t xml:space="preserve">to update a program with  invalid values in request body </t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>to update a program with  invalid program Description</t>
+  </si>
+  <si>
+    <t>to update a program status</t>
+  </si>
+  <si>
+    <t>to delete a program with valid programName</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>deletebyprogname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>/{programName}</t>
+    </r>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">200 Ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>status with message</t>
+    </r>
+  </si>
+  <si>
+    <t>to delete a program with valid LMS API,invalid programName</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>deletebyprogname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>/{invalidprogramName}</t>
+    </r>
+  </si>
+  <si>
+    <t>to delete a program name without Authorization</t>
+  </si>
+  <si>
+    <t>to delete a program with valid program ID</t>
+  </si>
+  <si>
+    <t>/deletebyprogid/{programId}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Admin receives </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>200 Ok</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> status with message</t>
+    </r>
+  </si>
+  <si>
+    <t>to delete a program with valid LMS API,invalid program ID</t>
+  </si>
+  <si>
+    <t>/deletebyprogid/{invalidprogramId}</t>
+  </si>
+  <si>
+    <t>to delete a program id without Authorization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,8 +1153,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,8 +1378,62 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFD0E0E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
+        <bgColor rgb="FFD5A6BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -606,6 +1548,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -652,9 +1657,91 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1033,7 +2120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S1" sqref="S1:X2"/>
     </sheetView>
   </sheetViews>
@@ -1168,12 +2255,1208 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994B6AFB-9E1D-4AFE-8F21-B4A585802674}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <v>404</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4">
+        <v>405</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5">
+        <v>401</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7">
+        <v>404</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8">
+        <v>404</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9">
+        <v>401</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10">
+        <v>404</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11">
+        <v>200</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12">
+        <v>404</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>405</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>401</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4C347-1F4A-491D-B34F-C7324167FC7B}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3">
+        <v>404</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4">
+        <v>10001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4">
+        <v>400</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5">
+        <v>400</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6">
+        <v>404</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7">
+        <v>405</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8">
+        <v>401</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9">
+        <v>200</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10">
+        <v>404</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11">
+        <v>400</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12">
+        <v>400</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>110101</v>
+      </c>
+      <c r="H13" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13">
+        <v>400</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" t="s">
+        <v>146</v>
+      </c>
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14">
+        <v>200</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15">
+        <v>401</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A39390C-1AEE-47C3-AD9D-AFD7CBB022EB}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <v>404</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4">
+        <v>401</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>404</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7">
+        <v>401</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47472022-1CAD-4FAF-B541-DF8D1C0AD1B1}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>16223</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93478661-72DF-41CC-A240-74127DBE3ACE}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>89463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C4C00C-4EB8-4299-B147-4732EC8B8FC8}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFE32FC-9E74-4324-9BC0-13F8F9AFBD45}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,12 +3524,84 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A270C26-81B4-4C77-A071-4D7CB6303311}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE306FB-861C-482C-ABBD-7FB7A32DC6C9}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A270C26-81B4-4C77-A071-4D7CB6303311}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +3636,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -1290,10 +3645,439 @@
         <v>31</v>
       </c>
       <c r="E2">
-        <v>16614</v>
+        <v>16248</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3">
+        <v>77777</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CBF0E2-5F5A-425D-9C86-E4ED1DAEE878}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>8568</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>16248</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C948EEDA-9B8B-4A9F-8FB2-C74E08823537}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="39.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="7">
+        <v>201</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="7">
+        <v>201</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="7">
+        <v>401</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="7">
+        <v>404</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="7">
+        <v>400</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="7">
+        <v>405</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="5">
+        <v>56798</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="7">
+        <v>400</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="7">
+        <v>400</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="11">
+        <v>400</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user module merged code for data driven -By Vani
</commit_message>
<xml_diff>
--- a/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
+++ b/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef72ffeab5838379/Desktop/Test Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team6_RestAssuredAPI\Users\senth\eclipse-workspace\Team6_Phase2_LMSAPIRestAssured\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{4FE9F826-4508-4007-9AA4-54A2112DD4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046BF60B-6792-4B92-B3F0-F9B0E640BC56}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF74C1E-A014-47E0-B997-D9FF5DE6ECF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
   <si>
     <t>userComments</t>
   </si>
@@ -179,13 +179,88 @@
   </si>
   <si>
     <t>INACTIVE</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>DigitalDragons</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>H1B</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/testing</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>TestDatanew</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>BTECH</t>
+  </si>
+  <si>
+    <t>Lastn</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/testdata</t>
+  </si>
+  <si>
+    <t>ATLANTA</t>
+  </si>
+  <si>
+    <t>qweN</t>
+  </si>
+  <si>
+    <t>middleN</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +414,21 @@
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF467886"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -638,7 +728,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -682,14 +772,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -724,10 +821,12 @@
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="44" xr:uid="{649120B8-1490-4FFA-8B63-C376AA98B509}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{98A04C51-BC0E-4D3C-B211-83EE3F381ACE}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1064,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,203 +1263,372 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="4">
+        <v>9210002622</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U2">
-        <v>16224</v>
-      </c>
-      <c r="V2">
-        <v>8652</v>
-      </c>
-      <c r="W2" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6368665333</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3">
-        <v>16210</v>
-      </c>
-      <c r="V3">
-        <v>8465</v>
-      </c>
-      <c r="W3" t="s">
-        <v>52</v>
-      </c>
+      <c r="P3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" t="s">
-        <v>28</v>
-      </c>
+      <c r="A4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6985749462</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" t="s">
-        <v>28</v>
-      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="5">
+        <v>4800475853</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
-        <v>34</v>
+      <c r="R6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" t="s">
+        <v>26</v>
       </c>
       <c r="T6" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="U6">
+        <v>16224</v>
+      </c>
+      <c r="V6">
+        <v>8652</v>
+      </c>
+      <c r="W6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" t="s">
+        <v>25</v>
       </c>
       <c r="T7" t="s">
         <v>27</v>
       </c>
+      <c r="U7">
+        <v>16210</v>
+      </c>
+      <c r="V7">
+        <v>8465</v>
+      </c>
+      <c r="W7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>38</v>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" t="s">
+        <v>29</v>
       </c>
       <c r="T8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" t="s">
+        <v>29</v>
       </c>
       <c r="T9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I10" s="2" t="s">
-        <v>42</v>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L11" t="s">
         <v>35</v>
       </c>
       <c r="T11" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1368,26 +1636,99 @@
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="J12" t="s">
         <v>32</v>
       </c>
       <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
+      <c r="T12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+      <c r="T14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="I15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T16" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I10" r:id="rId1" xr:uid="{D1E8CED3-8527-4B13-B10B-32F37A62C7C2}"/>
-    <hyperlink ref="I11" r:id="rId2" xr:uid="{44F1ABA1-50CD-4F49-93FA-03336969ED94}"/>
-    <hyperlink ref="L12" r:id="rId3" xr:uid="{CB113984-7A0E-47F4-97FF-DB753E79EA2B}"/>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{D1E8CED3-8527-4B13-B10B-32F37A62C7C2}"/>
+    <hyperlink ref="I15" r:id="rId2" xr:uid="{44F1ABA1-50CD-4F49-93FA-03336969ED94}"/>
+    <hyperlink ref="L16" r:id="rId3" xr:uid="{CB113984-7A0E-47F4-97FF-DB753E79EA2B}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{6779FF24-9CC0-4354-B09B-2FB84A70080C}"/>
+    <hyperlink ref="L2" r:id="rId8" xr:uid="{C4D3C0FD-36B6-4D34-8345-FDD95F630ED4}"/>
+    <hyperlink ref="L3" r:id="rId9" xr:uid="{2AD9F153-5103-4825-A5D3-D34F8AFE1871}"/>
+    <hyperlink ref="L4" r:id="rId10" xr:uid="{46351CB0-0DD7-4A59-99E0-D659B8BD93E4}"/>
+    <hyperlink ref="L5" r:id="rId11" xr:uid="{0CB5B618-FF2C-46F5-AD70-CE7686BCD933}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final merged code- By vani
</commit_message>
<xml_diff>
--- a/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
+++ b/Users/senth/eclipse-workspace/Team6_Phase2_LMSAPIRestAssured/src/test/resources/Test_Data/LMS_valid_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team6_RestAssuredAPI\Users\senth\eclipse-workspace\Team6_Phase2_LMSAPIRestAssured\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF74C1E-A014-47E0-B997-D9FF5DE6ECF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF50BCCF-365E-452B-8BC2-8ED04B069C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,16 +244,16 @@
     <t>middleN</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
+    <t>test1@gmail.comcom</t>
+  </si>
+  <si>
+    <t>test2@gmail.comcom</t>
+  </si>
+  <si>
+    <t>test3@gmail.comcom</t>
+  </si>
+  <si>
+    <t>test4@gmail.comcom</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1299,7 @@
         <v>73</v>
       </c>
       <c r="N2" s="4">
-        <v>9210002622</v>
+        <v>9999002622</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>32</v>
@@ -1359,7 +1359,7 @@
         <v>57</v>
       </c>
       <c r="N3" s="4">
-        <v>6368665333</v>
+        <v>6368666733</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>17</v>
@@ -1419,7 +1419,7 @@
         <v>57</v>
       </c>
       <c r="N4" s="4">
-        <v>6985749462</v>
+        <v>6985749962</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>17</v>
@@ -1477,7 +1477,7 @@
         <v>57</v>
       </c>
       <c r="N5" s="5">
-        <v>4800475853</v>
+        <v>4866475853</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>17</v>

</xml_diff>